<commit_message>
Work in process. Reorder loops. Maybe dataframe~ to materialID, type, thickness
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
+++ b/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>Material ID</t>
   </si>
@@ -174,9 +174,6 @@
     <t>643, 125, 77</t>
   </si>
   <si>
-    <t>two layers</t>
-  </si>
-  <si>
     <t>587, 125, 705</t>
   </si>
   <si>
@@ -184,6 +181,51 @@
   </si>
   <si>
     <t>Board is accurate</t>
+  </si>
+  <si>
+    <t>25, 50, 100</t>
+  </si>
+  <si>
+    <t>Provided dim.[mm]</t>
+  </si>
+  <si>
+    <t>25, 30, 50, 80</t>
+  </si>
+  <si>
+    <t>40, 60, 80, 100</t>
+  </si>
+  <si>
+    <t>30, 50, 80</t>
+  </si>
+  <si>
+    <t>60, 80, 100</t>
+  </si>
+  <si>
+    <t>45, 75, 95, 115, 140</t>
+  </si>
+  <si>
+    <t>20, 45, 65, 80, 90, 110</t>
+  </si>
+  <si>
+    <t>two layers (K118)</t>
+  </si>
+  <si>
+    <t>70, 95, 120</t>
+  </si>
+  <si>
+    <t>45, 70, 95, 120, 145, 195, 245</t>
+  </si>
+  <si>
+    <t>100, 120, 140, 160</t>
+  </si>
+  <si>
+    <t>120, 140, 160, 180, 200, 220, 240, 260, 280, 300</t>
+  </si>
+  <si>
+    <t>25, 35, 50, 75, 100</t>
+  </si>
+  <si>
+    <t>60, 80, 100, 120</t>
   </si>
 </sst>
 </file>
@@ -540,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,11 +593,12 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,13 +609,16 @@
         <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -582,11 +628,14 @@
       <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -594,13 +643,16 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -608,13 +660,16 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -622,14 +677,17 @@
         <v>6</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -639,11 +697,14 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -653,13 +714,16 @@
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D7" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -667,16 +731,19 @@
       <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -684,14 +751,17 @@
       <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -701,11 +771,14 @@
       <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -715,14 +788,17 @@
       <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -732,11 +808,14 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
@@ -746,14 +825,17 @@
       <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -763,14 +845,17 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>
@@ -781,6 +866,9 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -813,7 +901,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" display="http://www.conservationtech.ie/view-cats.php?prod_id=179 "/>
+    <hyperlink ref="F7" r:id="rId1" display="http://www.conservationtech.ie/view-cats.php?prod_id=179 "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
Still errors but full functionality is nearby. The complex looping might be lightened with change_layer_width rather than change_layer_widths.
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
+++ b/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Material ID</t>
   </si>
@@ -135,15 +135,9 @@
     <t>39, 125, 705</t>
   </si>
   <si>
-    <t>731, 599, 12</t>
-  </si>
-  <si>
     <t>+ vapour barrier EPS 1450/0.035/30-70 ID material 1500/0.036/96</t>
   </si>
   <si>
-    <t>644, 599, 12</t>
-  </si>
-  <si>
     <t>730, 599, 12</t>
   </si>
   <si>
@@ -153,18 +147,12 @@
     <t>Rockwool</t>
   </si>
   <si>
-    <t>+ vapour barrier Isover PBM 032</t>
-  </si>
-  <si>
     <t xml:space="preserve">+ vapour barrier Flexibatts 37 </t>
   </si>
   <si>
     <t>WoodWoolLightBuildingBoard</t>
   </si>
   <si>
-    <t>277, 599, 12</t>
-  </si>
-  <si>
     <t>ISOVER</t>
   </si>
   <si>
@@ -186,9 +174,6 @@
     <t>25, 50, 100</t>
   </si>
   <si>
-    <t>Provided dim.[mm]</t>
-  </si>
-  <si>
     <t>25, 30, 50, 80</t>
   </si>
   <si>
@@ -226,6 +211,33 @@
   </si>
   <si>
     <t>60, 80, 100, 120</t>
+  </si>
+  <si>
+    <t>Insulation dim.[mm]</t>
+  </si>
+  <si>
+    <t>Finish dim.[mm]</t>
+  </si>
+  <si>
+    <t>Detail dim.[mm]</t>
+  </si>
+  <si>
+    <t>Swisspor</t>
+  </si>
+  <si>
+    <t>+ vapour barrier Isover PBM 032 https://www.youtube.com/watch?v=dnj4MQkCsLY</t>
+  </si>
+  <si>
+    <t>Vapour barrier</t>
+  </si>
+  <si>
+    <t>644, 599</t>
+  </si>
+  <si>
+    <t>731, 599</t>
+  </si>
+  <si>
+    <t>276, 599</t>
   </si>
 </sst>
 </file>
@@ -582,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,12 +605,13 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,16 +622,25 @@
         <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -629,65 +651,109 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
       <c r="D3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
       <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
       <c r="D5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="3">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -698,13 +764,22 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -715,15 +790,24 @@
         <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -732,18 +816,27 @@
         <v>19</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -752,18 +845,27 @@
         <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="5">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -772,33 +874,49 @@
         <v>14</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -809,35 +927,51 @@
         <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E12" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="F13" s="5">
+        <v>22</v>
+      </c>
+      <c r="G13" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I13" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -846,29 +980,42 @@
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I14" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="G15" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>20</v>
       </c>
     </row>
@@ -901,7 +1048,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" display="http://www.conservationtech.ie/view-cats.php?prod_id=179 "/>
+    <hyperlink ref="I7" r:id="rId1" display="http://www.conservationtech.ie/view-cats.php?prod_id=179 "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>

</xml_diff>

<commit_message>
created better design info
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
+++ b/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
@@ -597,18 +597,20 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fixed problems with null in Delphin output files
</commit_message>
<xml_diff>
--- a/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
+++ b/delphin_6_automation/sampling/input_files/InsulationSystems.xlsx
@@ -622,7 +622,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +881,9 @@
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1145,9 +1147,6 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24">
-        <v>154</v>
-      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>

</xml_diff>